<commit_message>
Finalizando o módulo 4
</commit_message>
<xml_diff>
--- a/Modulo 4 - Mais tópicos de edição e formatação/aula-congelamento-protecao.xlsx
+++ b/Modulo 4 - Mais tópicos de edição e formatação/aula-congelamento-protecao.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nelio\Google Drive\Cursos online\Curso_Excel\04 Mais tópicos de edição e formatação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felipe\Desktop\Curso Excel\Modulo 4 - Mais tópicos de edição e formatação\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9630" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Menu" sheetId="4" r:id="rId1"/>
     <sheet name="Cadastro" sheetId="5" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -286,7 +286,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0000"/>
   </numFmts>
@@ -636,7 +636,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -697,26 +697,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -729,6 +714,42 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -768,7 +789,7 @@
         <xdr:cNvPr id="2" name="Retângulo: Cantos Superiores, Um Arredondado e Um Recortado 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D44425CF-D459-46F4-AEE1-C2BFC99935C2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D44425CF-D459-46F4-AEE1-C2BFC99935C2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -848,7 +869,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A92B70D-1891-489A-AD71-200252118BEF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A92B70D-1891-489A-AD71-200252118BEF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -925,7 +946,7 @@
         <xdr:cNvPr id="4" name="Retângulo: Cantos Superiores, Um Arredondado e Um Recortado 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F6F8A99-73EA-47E7-866F-232CE726F0BE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F6F8A99-73EA-47E7-866F-232CE726F0BE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1002,7 +1023,7 @@
         <xdr:cNvPr id="5" name="Retângulo: Cantos Superiores, Um Arredondado e Um Recortado 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04DD6E4B-3605-4BC0-BA76-5BF929399E3E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04DD6E4B-3605-4BC0-BA76-5BF929399E3E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1079,7 +1100,7 @@
         <xdr:cNvPr id="6" name="Retângulo: Cantos Superiores, Um Arredondado e Um Recortado 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59861F94-AF37-4415-989D-75866B16F2B5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59861F94-AF37-4415-989D-75866B16F2B5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1162,7 +1183,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F06A00D-B7F6-4EF2-A9C5-5628A837B16C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F06A00D-B7F6-4EF2-A9C5-5628A837B16C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1239,7 +1260,7 @@
         <xdr:cNvPr id="3" name="Retângulo: Cantos Superiores, Um Arredondado e Um Recortado 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E67EF430-9BAC-4DC8-8401-0C98D9096FE3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E67EF430-9BAC-4DC8-8401-0C98D9096FE3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1318,7 +1339,7 @@
         <xdr:cNvPr id="4" name="Retângulo: Cantos Superiores, Um Arredondado e Um Recortado 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60E7EC31-1DDE-418E-BD9A-1C7CA40496C0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60E7EC31-1DDE-418E-BD9A-1C7CA40496C0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1395,7 +1416,7 @@
         <xdr:cNvPr id="5" name="Retângulo: Cantos Superiores, Um Arredondado e Um Recortado 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01964716-4EAB-46C6-96AD-25F64AFD83B0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01964716-4EAB-46C6-96AD-25F64AFD83B0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1472,7 +1493,7 @@
         <xdr:cNvPr id="6" name="Retângulo: Cantos Superiores, Um Arredondado e Um Recortado 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B93A7A8-2556-40E8-9001-607F1CA08116}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B93A7A8-2556-40E8-9001-607F1CA08116}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2306,7 +2327,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.25" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2408,29 +2432,29 @@
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B5" s="28"/>
-      <c r="C5" s="36">
+      <c r="C5" s="42">
         <v>1</v>
       </c>
-      <c r="D5" s="37" t="s">
+      <c r="D5" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="E5" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="F5" s="37" t="s">
+      <c r="F5" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="37">
+      <c r="G5" s="43">
         <v>2012</v>
       </c>
-      <c r="H5" s="38" t="s">
+      <c r="H5" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="I5" s="39">
+      <c r="I5" s="36">
         <f ca="1">YEAR(TODAY())-G5</f>
-        <v>6</v>
-      </c>
-      <c r="J5" s="40"/>
+        <v>11</v>
+      </c>
+      <c r="J5" s="37"/>
       <c r="K5" s="34"/>
       <c r="L5" s="34"/>
       <c r="M5" s="34"/>
@@ -2439,29 +2463,29 @@
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B6" s="28"/>
-      <c r="C6" s="41">
+      <c r="C6" s="45">
         <v>2</v>
       </c>
-      <c r="D6" s="34" t="s">
+      <c r="D6" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="34" t="s">
+      <c r="E6" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="F6" s="34" t="s">
+      <c r="F6" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="G6" s="34">
+      <c r="G6" s="46">
         <v>2006</v>
       </c>
-      <c r="H6" s="35" t="s">
+      <c r="H6" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="I6" s="39">
+      <c r="I6" s="36">
         <f t="shared" ref="I6:I44" ca="1" si="0">YEAR(TODAY())-G6</f>
-        <v>12</v>
-      </c>
-      <c r="J6" s="40"/>
+        <v>17</v>
+      </c>
+      <c r="J6" s="37"/>
       <c r="K6" s="34"/>
       <c r="L6" s="34"/>
       <c r="M6" s="34"/>
@@ -2470,29 +2494,29 @@
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B7" s="28"/>
-      <c r="C7" s="41">
+      <c r="C7" s="45">
         <v>3</v>
       </c>
-      <c r="D7" s="34" t="s">
+      <c r="D7" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="34" t="s">
+      <c r="E7" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="F7" s="34" t="s">
+      <c r="F7" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="G7" s="34">
+      <c r="G7" s="46">
         <v>2007</v>
       </c>
-      <c r="H7" s="35" t="s">
+      <c r="H7" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="I7" s="39">
+      <c r="I7" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="J7" s="40"/>
+        <v>16</v>
+      </c>
+      <c r="J7" s="37"/>
       <c r="K7" s="34"/>
       <c r="L7" s="34"/>
       <c r="M7" s="34"/>
@@ -2501,29 +2525,29 @@
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B8" s="28"/>
-      <c r="C8" s="41">
+      <c r="C8" s="45">
         <v>4</v>
       </c>
-      <c r="D8" s="34" t="s">
+      <c r="D8" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="34" t="s">
+      <c r="E8" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="F8" s="34" t="s">
+      <c r="F8" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="G8" s="34">
+      <c r="G8" s="46">
         <v>2007</v>
       </c>
-      <c r="H8" s="35" t="s">
+      <c r="H8" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="I8" s="39">
+      <c r="I8" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="J8" s="40"/>
+        <v>16</v>
+      </c>
+      <c r="J8" s="37"/>
       <c r="K8" s="34"/>
       <c r="L8" s="34"/>
       <c r="M8" s="34"/>
@@ -2532,29 +2556,29 @@
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B9" s="28"/>
-      <c r="C9" s="41">
+      <c r="C9" s="45">
         <v>5</v>
       </c>
-      <c r="D9" s="34" t="s">
+      <c r="D9" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="34" t="s">
+      <c r="E9" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="F9" s="34" t="s">
+      <c r="F9" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="G9" s="34">
+      <c r="G9" s="46">
         <v>2008</v>
       </c>
-      <c r="H9" s="35" t="s">
+      <c r="H9" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="I9" s="39">
+      <c r="I9" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="J9" s="40"/>
+        <v>15</v>
+      </c>
+      <c r="J9" s="37"/>
       <c r="K9" s="34"/>
       <c r="L9" s="34"/>
       <c r="M9" s="34"/>
@@ -2563,29 +2587,29 @@
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B10" s="28"/>
-      <c r="C10" s="41">
+      <c r="C10" s="45">
         <v>6</v>
       </c>
-      <c r="D10" s="34" t="s">
+      <c r="D10" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="34" t="s">
+      <c r="E10" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="F10" s="34" t="s">
+      <c r="F10" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="G10" s="34">
+      <c r="G10" s="46">
         <v>2008</v>
       </c>
-      <c r="H10" s="35" t="s">
+      <c r="H10" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="I10" s="39">
+      <c r="I10" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="J10" s="40"/>
+        <v>15</v>
+      </c>
+      <c r="J10" s="37"/>
       <c r="K10" s="34"/>
       <c r="L10" s="34"/>
       <c r="M10" s="34"/>
@@ -2594,29 +2618,29 @@
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B11" s="28"/>
-      <c r="C11" s="41">
+      <c r="C11" s="45">
         <v>7</v>
       </c>
-      <c r="D11" s="34" t="s">
+      <c r="D11" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="34" t="s">
+      <c r="E11" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="F11" s="34" t="s">
+      <c r="F11" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="G11" s="34">
+      <c r="G11" s="46">
         <v>2008</v>
       </c>
-      <c r="H11" s="35" t="s">
+      <c r="H11" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="I11" s="39">
+      <c r="I11" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="J11" s="40"/>
+        <v>15</v>
+      </c>
+      <c r="J11" s="37"/>
       <c r="K11" s="34"/>
       <c r="L11" s="34"/>
       <c r="M11" s="34"/>
@@ -2625,29 +2649,29 @@
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B12" s="28"/>
-      <c r="C12" s="41">
+      <c r="C12" s="45">
         <v>8</v>
       </c>
-      <c r="D12" s="34" t="s">
+      <c r="D12" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="34" t="s">
+      <c r="E12" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="F12" s="34" t="s">
+      <c r="F12" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="G12" s="34">
+      <c r="G12" s="46">
         <v>2008</v>
       </c>
-      <c r="H12" s="35" t="s">
+      <c r="H12" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="I12" s="39">
+      <c r="I12" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="J12" s="40"/>
+        <v>15</v>
+      </c>
+      <c r="J12" s="37"/>
       <c r="K12" s="34"/>
       <c r="L12" s="34"/>
       <c r="M12" s="34"/>
@@ -2656,29 +2680,29 @@
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B13" s="28"/>
-      <c r="C13" s="41">
+      <c r="C13" s="45">
         <v>9</v>
       </c>
-      <c r="D13" s="34" t="s">
+      <c r="D13" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="34" t="s">
+      <c r="E13" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="34" t="s">
+      <c r="F13" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="G13" s="34">
+      <c r="G13" s="46">
         <v>2009</v>
       </c>
-      <c r="H13" s="35" t="s">
+      <c r="H13" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="I13" s="39">
+      <c r="I13" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="J13" s="40"/>
+        <v>14</v>
+      </c>
+      <c r="J13" s="37"/>
       <c r="K13" s="34"/>
       <c r="L13" s="34"/>
       <c r="M13" s="34"/>
@@ -2687,29 +2711,29 @@
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B14" s="28"/>
-      <c r="C14" s="41">
+      <c r="C14" s="45">
         <v>10</v>
       </c>
-      <c r="D14" s="34" t="s">
+      <c r="D14" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="34" t="s">
+      <c r="E14" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="F14" s="34" t="s">
+      <c r="F14" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="G14" s="34">
+      <c r="G14" s="46">
         <v>2009</v>
       </c>
-      <c r="H14" s="35" t="s">
+      <c r="H14" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="I14" s="39">
+      <c r="I14" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="J14" s="40"/>
+        <v>14</v>
+      </c>
+      <c r="J14" s="37"/>
       <c r="K14" s="34"/>
       <c r="L14" s="34"/>
       <c r="M14" s="34"/>
@@ -2718,29 +2742,29 @@
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B15" s="28"/>
-      <c r="C15" s="41">
+      <c r="C15" s="45">
         <v>11</v>
       </c>
-      <c r="D15" s="34" t="s">
+      <c r="D15" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="34" t="s">
+      <c r="E15" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="F15" s="34" t="s">
+      <c r="F15" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="G15" s="34">
+      <c r="G15" s="46">
         <v>2009</v>
       </c>
-      <c r="H15" s="35" t="s">
+      <c r="H15" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="I15" s="39">
+      <c r="I15" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="J15" s="40"/>
+        <v>14</v>
+      </c>
+      <c r="J15" s="37"/>
       <c r="K15" s="34"/>
       <c r="L15" s="34"/>
       <c r="M15" s="34"/>
@@ -2749,29 +2773,29 @@
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B16" s="28"/>
-      <c r="C16" s="41">
+      <c r="C16" s="45">
         <v>12</v>
       </c>
-      <c r="D16" s="34" t="s">
+      <c r="D16" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="34" t="s">
+      <c r="E16" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="F16" s="34" t="s">
+      <c r="F16" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="G16" s="34">
+      <c r="G16" s="46">
         <v>2010</v>
       </c>
-      <c r="H16" s="35" t="s">
+      <c r="H16" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="I16" s="39">
+      <c r="I16" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="J16" s="40"/>
+        <v>13</v>
+      </c>
+      <c r="J16" s="37"/>
       <c r="K16" s="34"/>
       <c r="L16" s="34"/>
       <c r="M16" s="34"/>
@@ -2780,29 +2804,29 @@
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B17" s="28"/>
-      <c r="C17" s="41">
+      <c r="C17" s="45">
         <v>13</v>
       </c>
-      <c r="D17" s="34" t="s">
+      <c r="D17" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="34" t="s">
+      <c r="E17" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="F17" s="34" t="s">
+      <c r="F17" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="G17" s="34">
+      <c r="G17" s="46">
         <v>2010</v>
       </c>
-      <c r="H17" s="35" t="s">
+      <c r="H17" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="I17" s="39">
+      <c r="I17" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="J17" s="40"/>
+        <v>13</v>
+      </c>
+      <c r="J17" s="37"/>
       <c r="K17" s="34"/>
       <c r="L17" s="34"/>
       <c r="M17" s="34"/>
@@ -2811,29 +2835,29 @@
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B18" s="28"/>
-      <c r="C18" s="41">
+      <c r="C18" s="45">
         <v>14</v>
       </c>
-      <c r="D18" s="34" t="s">
+      <c r="D18" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="E18" s="34" t="s">
+      <c r="E18" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="F18" s="34" t="s">
+      <c r="F18" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="G18" s="34">
+      <c r="G18" s="46">
         <v>2010</v>
       </c>
-      <c r="H18" s="35" t="s">
+      <c r="H18" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="I18" s="39">
+      <c r="I18" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="J18" s="40"/>
+        <v>13</v>
+      </c>
+      <c r="J18" s="37"/>
       <c r="K18" s="34"/>
       <c r="L18" s="34"/>
       <c r="M18" s="34"/>
@@ -2842,29 +2866,29 @@
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B19" s="28"/>
-      <c r="C19" s="41">
+      <c r="C19" s="45">
         <v>15</v>
       </c>
-      <c r="D19" s="34" t="s">
+      <c r="D19" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="34" t="s">
+      <c r="E19" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="F19" s="34" t="s">
+      <c r="F19" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="G19" s="34">
+      <c r="G19" s="46">
         <v>2011</v>
       </c>
-      <c r="H19" s="35" t="s">
+      <c r="H19" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="I19" s="39">
+      <c r="I19" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="J19" s="40"/>
+        <v>12</v>
+      </c>
+      <c r="J19" s="37"/>
       <c r="K19" s="34"/>
       <c r="L19" s="34"/>
       <c r="M19" s="34"/>
@@ -2873,29 +2897,29 @@
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B20" s="28"/>
-      <c r="C20" s="41">
+      <c r="C20" s="45">
         <v>16</v>
       </c>
-      <c r="D20" s="34" t="s">
+      <c r="D20" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="E20" s="34" t="s">
+      <c r="E20" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="F20" s="34" t="s">
+      <c r="F20" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="G20" s="34">
+      <c r="G20" s="46">
         <v>2011</v>
       </c>
-      <c r="H20" s="35" t="s">
+      <c r="H20" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="I20" s="39">
+      <c r="I20" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="J20" s="40"/>
+        <v>12</v>
+      </c>
+      <c r="J20" s="37"/>
       <c r="K20" s="34"/>
       <c r="L20" s="34"/>
       <c r="M20" s="34"/>
@@ -2904,29 +2928,29 @@
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B21" s="28"/>
-      <c r="C21" s="41">
+      <c r="C21" s="45">
         <v>17</v>
       </c>
-      <c r="D21" s="34" t="s">
+      <c r="D21" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="E21" s="34" t="s">
+      <c r="E21" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="F21" s="34" t="s">
+      <c r="F21" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="G21" s="34">
+      <c r="G21" s="46">
         <v>2011</v>
       </c>
-      <c r="H21" s="35" t="s">
+      <c r="H21" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="I21" s="39">
+      <c r="I21" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="J21" s="40"/>
+        <v>12</v>
+      </c>
+      <c r="J21" s="37"/>
       <c r="K21" s="34"/>
       <c r="L21" s="34"/>
       <c r="M21" s="34"/>
@@ -2935,29 +2959,29 @@
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B22" s="28"/>
-      <c r="C22" s="41">
+      <c r="C22" s="45">
         <v>18</v>
       </c>
-      <c r="D22" s="34" t="s">
+      <c r="D22" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="E22" s="34" t="s">
+      <c r="E22" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="F22" s="34" t="s">
+      <c r="F22" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="G22" s="34">
+      <c r="G22" s="46">
         <v>2012</v>
       </c>
-      <c r="H22" s="35" t="s">
+      <c r="H22" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="I22" s="39">
+      <c r="I22" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="J22" s="40"/>
+        <v>11</v>
+      </c>
+      <c r="J22" s="37"/>
       <c r="K22" s="34"/>
       <c r="L22" s="34"/>
       <c r="M22" s="34"/>
@@ -2966,29 +2990,29 @@
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B23" s="28"/>
-      <c r="C23" s="41">
+      <c r="C23" s="45">
         <v>19</v>
       </c>
-      <c r="D23" s="34" t="s">
+      <c r="D23" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="E23" s="34" t="s">
+      <c r="E23" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="F23" s="34" t="s">
+      <c r="F23" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="G23" s="34">
+      <c r="G23" s="46">
         <v>2012</v>
       </c>
-      <c r="H23" s="35" t="s">
+      <c r="H23" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="I23" s="39">
+      <c r="I23" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="J23" s="40"/>
+        <v>11</v>
+      </c>
+      <c r="J23" s="37"/>
       <c r="K23" s="34"/>
       <c r="L23" s="34"/>
       <c r="M23" s="34"/>
@@ -2997,29 +3021,29 @@
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B24" s="28"/>
-      <c r="C24" s="41">
+      <c r="C24" s="45">
         <v>20</v>
       </c>
-      <c r="D24" s="34" t="s">
+      <c r="D24" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="E24" s="34" t="s">
+      <c r="E24" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="F24" s="34" t="s">
+      <c r="F24" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="G24" s="34">
+      <c r="G24" s="46">
         <v>2013</v>
       </c>
-      <c r="H24" s="35" t="s">
+      <c r="H24" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="I24" s="39">
+      <c r="I24" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="J24" s="40"/>
+        <v>10</v>
+      </c>
+      <c r="J24" s="37"/>
       <c r="K24" s="34"/>
       <c r="L24" s="34"/>
       <c r="M24" s="34"/>
@@ -3028,29 +3052,29 @@
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B25" s="28"/>
-      <c r="C25" s="41">
+      <c r="C25" s="45">
         <v>21</v>
       </c>
-      <c r="D25" s="34" t="s">
+      <c r="D25" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="E25" s="34" t="s">
+      <c r="E25" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="F25" s="34" t="s">
+      <c r="F25" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="G25" s="34">
+      <c r="G25" s="46">
         <v>2013</v>
       </c>
-      <c r="H25" s="35" t="s">
+      <c r="H25" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="I25" s="39">
+      <c r="I25" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="J25" s="40"/>
+        <v>10</v>
+      </c>
+      <c r="J25" s="37"/>
       <c r="K25" s="34"/>
       <c r="L25" s="34"/>
       <c r="M25" s="34"/>
@@ -3059,29 +3083,29 @@
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B26" s="28"/>
-      <c r="C26" s="41">
+      <c r="C26" s="45">
         <v>22</v>
       </c>
-      <c r="D26" s="34" t="s">
+      <c r="D26" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="34" t="s">
+      <c r="E26" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="F26" s="34" t="s">
+      <c r="F26" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="G26" s="34">
+      <c r="G26" s="46">
         <v>2013</v>
       </c>
-      <c r="H26" s="35" t="s">
+      <c r="H26" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="I26" s="39">
+      <c r="I26" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="J26" s="40"/>
+        <v>10</v>
+      </c>
+      <c r="J26" s="37"/>
       <c r="K26" s="34"/>
       <c r="L26" s="34"/>
       <c r="M26" s="34"/>
@@ -3090,29 +3114,29 @@
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B27" s="28"/>
-      <c r="C27" s="41">
+      <c r="C27" s="45">
         <v>23</v>
       </c>
-      <c r="D27" s="34" t="s">
+      <c r="D27" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="E27" s="34" t="s">
+      <c r="E27" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="F27" s="34" t="s">
+      <c r="F27" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="G27" s="34">
+      <c r="G27" s="46">
         <v>2013</v>
       </c>
-      <c r="H27" s="35" t="s">
+      <c r="H27" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="I27" s="39">
+      <c r="I27" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="J27" s="40"/>
+        <v>10</v>
+      </c>
+      <c r="J27" s="37"/>
       <c r="K27" s="34"/>
       <c r="L27" s="34"/>
       <c r="M27" s="34"/>
@@ -3121,29 +3145,29 @@
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B28" s="28"/>
-      <c r="C28" s="41">
+      <c r="C28" s="45">
         <v>24</v>
       </c>
-      <c r="D28" s="34" t="s">
+      <c r="D28" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="E28" s="34" t="s">
+      <c r="E28" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="F28" s="34" t="s">
+      <c r="F28" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="G28" s="34">
+      <c r="G28" s="46">
         <v>2013</v>
       </c>
-      <c r="H28" s="35" t="s">
+      <c r="H28" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="I28" s="39">
+      <c r="I28" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="J28" s="40"/>
+        <v>10</v>
+      </c>
+      <c r="J28" s="37"/>
       <c r="K28" s="34"/>
       <c r="L28" s="34"/>
       <c r="M28" s="34"/>
@@ -3152,29 +3176,29 @@
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B29" s="28"/>
-      <c r="C29" s="41">
+      <c r="C29" s="45">
         <v>25</v>
       </c>
-      <c r="D29" s="34" t="s">
+      <c r="D29" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="E29" s="34" t="s">
+      <c r="E29" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="F29" s="34" t="s">
+      <c r="F29" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="G29" s="34">
+      <c r="G29" s="46">
         <v>2013</v>
       </c>
-      <c r="H29" s="35" t="s">
+      <c r="H29" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="I29" s="39">
+      <c r="I29" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="J29" s="40"/>
+        <v>10</v>
+      </c>
+      <c r="J29" s="37"/>
       <c r="K29" s="34"/>
       <c r="L29" s="34"/>
       <c r="M29" s="34"/>
@@ -3183,29 +3207,29 @@
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B30" s="28"/>
-      <c r="C30" s="41">
+      <c r="C30" s="45">
         <v>26</v>
       </c>
-      <c r="D30" s="34" t="s">
+      <c r="D30" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="E30" s="34" t="s">
+      <c r="E30" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="F30" s="34" t="s">
+      <c r="F30" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="G30" s="34">
+      <c r="G30" s="46">
         <v>2014</v>
       </c>
-      <c r="H30" s="35" t="s">
+      <c r="H30" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="I30" s="39">
+      <c r="I30" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="J30" s="40"/>
+        <v>9</v>
+      </c>
+      <c r="J30" s="37"/>
       <c r="K30" s="34"/>
       <c r="L30" s="34"/>
       <c r="M30" s="34"/>
@@ -3214,29 +3238,29 @@
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B31" s="28"/>
-      <c r="C31" s="41">
+      <c r="C31" s="45">
         <v>27</v>
       </c>
-      <c r="D31" s="34" t="s">
+      <c r="D31" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="E31" s="34" t="s">
+      <c r="E31" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="F31" s="34" t="s">
+      <c r="F31" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="G31" s="34">
+      <c r="G31" s="46">
         <v>2014</v>
       </c>
-      <c r="H31" s="35" t="s">
+      <c r="H31" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="I31" s="39">
+      <c r="I31" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="J31" s="40"/>
+        <v>9</v>
+      </c>
+      <c r="J31" s="37"/>
       <c r="K31" s="34"/>
       <c r="L31" s="34"/>
       <c r="M31" s="34"/>
@@ -3245,29 +3269,29 @@
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B32" s="28"/>
-      <c r="C32" s="41">
+      <c r="C32" s="45">
         <v>28</v>
       </c>
-      <c r="D32" s="34" t="s">
+      <c r="D32" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="E32" s="34" t="s">
+      <c r="E32" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="F32" s="34" t="s">
+      <c r="F32" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="G32" s="34">
+      <c r="G32" s="46">
         <v>2015</v>
       </c>
-      <c r="H32" s="35" t="s">
+      <c r="H32" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="I32" s="39">
+      <c r="I32" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="J32" s="40"/>
+        <v>8</v>
+      </c>
+      <c r="J32" s="37"/>
       <c r="K32" s="34"/>
       <c r="L32" s="34"/>
       <c r="M32" s="34"/>
@@ -3276,29 +3300,29 @@
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B33" s="28"/>
-      <c r="C33" s="41">
+      <c r="C33" s="45">
         <v>29</v>
       </c>
-      <c r="D33" s="34" t="s">
+      <c r="D33" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="E33" s="34" t="s">
+      <c r="E33" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="F33" s="34" t="s">
+      <c r="F33" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="G33" s="34">
+      <c r="G33" s="46">
         <v>2016</v>
       </c>
-      <c r="H33" s="35" t="s">
+      <c r="H33" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="I33" s="39">
+      <c r="I33" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="J33" s="40"/>
+        <v>7</v>
+      </c>
+      <c r="J33" s="37"/>
       <c r="K33" s="34"/>
       <c r="L33" s="34"/>
       <c r="M33" s="34"/>
@@ -3307,29 +3331,29 @@
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B34" s="28"/>
-      <c r="C34" s="41">
+      <c r="C34" s="45">
         <v>30</v>
       </c>
-      <c r="D34" s="34" t="s">
+      <c r="D34" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="E34" s="34" t="s">
+      <c r="E34" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="F34" s="34" t="s">
+      <c r="F34" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="G34" s="34">
+      <c r="G34" s="46">
         <v>2016</v>
       </c>
-      <c r="H34" s="35" t="s">
+      <c r="H34" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="I34" s="39">
+      <c r="I34" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="J34" s="40"/>
+        <v>7</v>
+      </c>
+      <c r="J34" s="37"/>
       <c r="K34" s="34"/>
       <c r="L34" s="34"/>
       <c r="M34" s="34"/>
@@ -3338,29 +3362,29 @@
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B35" s="28"/>
-      <c r="C35" s="41">
+      <c r="C35" s="45">
         <v>31</v>
       </c>
-      <c r="D35" s="34" t="s">
+      <c r="D35" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="E35" s="34" t="s">
+      <c r="E35" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="F35" s="34" t="s">
+      <c r="F35" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="G35" s="34">
+      <c r="G35" s="46">
         <v>2016</v>
       </c>
-      <c r="H35" s="35" t="s">
+      <c r="H35" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="I35" s="39">
+      <c r="I35" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="J35" s="40"/>
+        <v>7</v>
+      </c>
+      <c r="J35" s="37"/>
       <c r="K35" s="34"/>
       <c r="L35" s="34"/>
       <c r="M35" s="34"/>
@@ -3369,29 +3393,29 @@
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B36" s="28"/>
-      <c r="C36" s="41">
+      <c r="C36" s="45">
         <v>32</v>
       </c>
-      <c r="D36" s="34" t="s">
+      <c r="D36" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="E36" s="34" t="s">
+      <c r="E36" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="F36" s="34" t="s">
+      <c r="F36" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="G36" s="34">
+      <c r="G36" s="46">
         <v>2016</v>
       </c>
-      <c r="H36" s="35" t="s">
+      <c r="H36" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="I36" s="39">
+      <c r="I36" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="J36" s="40"/>
+        <v>7</v>
+      </c>
+      <c r="J36" s="37"/>
       <c r="K36" s="34"/>
       <c r="L36" s="34"/>
       <c r="M36" s="34"/>
@@ -3400,29 +3424,29 @@
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B37" s="28"/>
-      <c r="C37" s="41">
+      <c r="C37" s="45">
         <v>33</v>
       </c>
-      <c r="D37" s="34" t="s">
+      <c r="D37" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="E37" s="34" t="s">
+      <c r="E37" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="F37" s="34" t="s">
+      <c r="F37" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="G37" s="34">
+      <c r="G37" s="46">
         <v>2017</v>
       </c>
-      <c r="H37" s="35" t="s">
+      <c r="H37" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="I37" s="39">
+      <c r="I37" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="J37" s="40"/>
+        <v>6</v>
+      </c>
+      <c r="J37" s="37"/>
       <c r="K37" s="34"/>
       <c r="L37" s="34"/>
       <c r="M37" s="34"/>
@@ -3431,29 +3455,29 @@
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B38" s="28"/>
-      <c r="C38" s="41">
+      <c r="C38" s="45">
         <v>34</v>
       </c>
-      <c r="D38" s="34" t="s">
+      <c r="D38" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="E38" s="34" t="s">
+      <c r="E38" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="F38" s="34" t="s">
+      <c r="F38" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="G38" s="34">
+      <c r="G38" s="46">
         <v>2017</v>
       </c>
-      <c r="H38" s="35" t="s">
+      <c r="H38" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="I38" s="39">
+      <c r="I38" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="J38" s="40"/>
+        <v>6</v>
+      </c>
+      <c r="J38" s="37"/>
       <c r="K38" s="34"/>
       <c r="L38" s="34"/>
       <c r="M38" s="34"/>
@@ -3462,29 +3486,29 @@
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B39" s="28"/>
-      <c r="C39" s="41">
+      <c r="C39" s="45">
         <v>35</v>
       </c>
-      <c r="D39" s="34" t="s">
+      <c r="D39" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="E39" s="34" t="s">
+      <c r="E39" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="F39" s="34" t="s">
+      <c r="F39" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="G39" s="34">
+      <c r="G39" s="46">
         <v>2017</v>
       </c>
-      <c r="H39" s="35" t="s">
+      <c r="H39" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="I39" s="39">
+      <c r="I39" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="J39" s="40"/>
+        <v>6</v>
+      </c>
+      <c r="J39" s="37"/>
       <c r="K39" s="34"/>
       <c r="L39" s="34"/>
       <c r="M39" s="34"/>
@@ -3493,29 +3517,29 @@
     </row>
     <row r="40" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B40" s="28"/>
-      <c r="C40" s="41">
+      <c r="C40" s="45">
         <v>36</v>
       </c>
-      <c r="D40" s="34" t="s">
+      <c r="D40" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="E40" s="34" t="s">
+      <c r="E40" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="F40" s="34" t="s">
+      <c r="F40" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="G40" s="34">
+      <c r="G40" s="46">
         <v>2017</v>
       </c>
-      <c r="H40" s="35" t="s">
+      <c r="H40" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="I40" s="39">
+      <c r="I40" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="J40" s="40"/>
+        <v>6</v>
+      </c>
+      <c r="J40" s="37"/>
       <c r="K40" s="34"/>
       <c r="L40" s="34"/>
       <c r="M40" s="34"/>
@@ -3524,29 +3548,29 @@
     </row>
     <row r="41" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B41" s="28"/>
-      <c r="C41" s="41">
+      <c r="C41" s="45">
         <v>37</v>
       </c>
-      <c r="D41" s="34" t="s">
+      <c r="D41" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="E41" s="34" t="s">
+      <c r="E41" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="F41" s="34" t="s">
+      <c r="F41" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="G41" s="34">
+      <c r="G41" s="46">
         <v>2017</v>
       </c>
-      <c r="H41" s="35" t="s">
+      <c r="H41" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="I41" s="39">
+      <c r="I41" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="J41" s="40"/>
+        <v>6</v>
+      </c>
+      <c r="J41" s="37"/>
       <c r="K41" s="34"/>
       <c r="L41" s="34"/>
       <c r="M41" s="34"/>
@@ -3555,29 +3579,29 @@
     </row>
     <row r="42" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B42" s="28"/>
-      <c r="C42" s="41">
+      <c r="C42" s="45">
         <v>38</v>
       </c>
-      <c r="D42" s="34" t="s">
+      <c r="D42" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="E42" s="34" t="s">
+      <c r="E42" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="F42" s="34" t="s">
+      <c r="F42" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="G42" s="34">
+      <c r="G42" s="46">
         <v>2017</v>
       </c>
-      <c r="H42" s="35" t="s">
+      <c r="H42" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="I42" s="39">
+      <c r="I42" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="J42" s="40"/>
+        <v>6</v>
+      </c>
+      <c r="J42" s="37"/>
       <c r="K42" s="34"/>
       <c r="L42" s="34"/>
       <c r="M42" s="34"/>
@@ -3586,29 +3610,29 @@
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B43" s="28"/>
-      <c r="C43" s="41">
+      <c r="C43" s="45">
         <v>39</v>
       </c>
-      <c r="D43" s="34" t="s">
+      <c r="D43" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="E43" s="34" t="s">
+      <c r="E43" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="F43" s="34" t="s">
+      <c r="F43" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="G43" s="34">
+      <c r="G43" s="46">
         <v>2018</v>
       </c>
-      <c r="H43" s="35" t="s">
+      <c r="H43" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="I43" s="39">
+      <c r="I43" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J43" s="40"/>
+        <v>5</v>
+      </c>
+      <c r="J43" s="37"/>
       <c r="K43" s="34"/>
       <c r="L43" s="34"/>
       <c r="M43" s="34"/>
@@ -3617,29 +3641,29 @@
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B44" s="28"/>
-      <c r="C44" s="42">
+      <c r="C44" s="48">
         <v>40</v>
       </c>
-      <c r="D44" s="43" t="s">
+      <c r="D44" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="E44" s="43" t="s">
+      <c r="E44" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="F44" s="43" t="s">
+      <c r="F44" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="G44" s="43">
+      <c r="G44" s="49">
         <v>2018</v>
       </c>
-      <c r="H44" s="44" t="s">
+      <c r="H44" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="I44" s="45">
+      <c r="I44" s="40">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J44" s="40"/>
+        <v>5</v>
+      </c>
+      <c r="J44" s="37"/>
       <c r="K44" s="34"/>
       <c r="L44" s="34"/>
       <c r="M44" s="34"/>
@@ -3647,24 +3671,25 @@
       <c r="O44" s="35"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B45" s="46"/>
-      <c r="C45" s="43"/>
-      <c r="D45" s="43"/>
-      <c r="E45" s="43"/>
-      <c r="F45" s="43"/>
-      <c r="G45" s="43"/>
-      <c r="H45" s="43"/>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43"/>
-      <c r="K45" s="43"/>
-      <c r="L45" s="43"/>
-      <c r="M45" s="43"/>
-      <c r="N45" s="43"/>
-      <c r="O45" s="44"/>
+      <c r="B45" s="41"/>
+      <c r="C45" s="38"/>
+      <c r="D45" s="38"/>
+      <c r="E45" s="38"/>
+      <c r="F45" s="38"/>
+      <c r="G45" s="38"/>
+      <c r="H45" s="38"/>
+      <c r="I45" s="38"/>
+      <c r="J45" s="38"/>
+      <c r="K45" s="38"/>
+      <c r="L45" s="38"/>
+      <c r="M45" s="38"/>
+      <c r="N45" s="38"/>
+      <c r="O45" s="39"/>
     </row>
     <row r="46" spans="2:15" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="47" spans="2:15" hidden="1" x14ac:dyDescent="0.2"/>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="fxzZM/qLOeQ8P2nxMB1WhqB6AE1jm09Q/yirqHzD65FBs0H0MheGjvZdx6/erSy6l+Ip1ofevWJ8hAV1HbCvhQ==" saltValue="3P8H3qkQrZMTirlUlzUEpg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <sortState ref="D5:G44">
     <sortCondition ref="G5:G44"/>
   </sortState>

</xml_diff>